<commit_message>
Centros geometricos da bateria e tanques
</commit_message>
<xml_diff>
--- a/Estabilidade/Centros_Geometricos.xlsx
+++ b/Estabilidade/Centros_Geometricos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projeto_Integrador_G6\Estabilidade\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alves\Desktop\Projeto_Integrador_G6\Estabilidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA6FBFA-F8AC-49A5-B2F4-9C6323814392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Origem</t>
   </si>
@@ -74,9 +75,6 @@
     <t>Bateria</t>
   </si>
   <si>
-    <t>Tanque Combustivel</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -117,12 +115,18 @@
   </si>
   <si>
     <t>Components</t>
+  </si>
+  <si>
+    <t>Tanque Combustivel asa direita</t>
+  </si>
+  <si>
+    <t>Tanque Combustivel asa esquerda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -229,11 +233,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -266,7 +281,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -304,7 +324,7 @@
         <xdr:cNvPr id="2" name="Imagem 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0437E8A4-EC7B-4CA9-995F-68716B93FCC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0437E8A4-EC7B-4CA9-995F-68716B93FCC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -595,41 +615,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="E1" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,10 +663,10 @@
         <v>7372.82</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -660,10 +680,10 @@
         <v>9529.07</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -677,10 +697,10 @@
         <v>5213.58</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -694,10 +714,10 @@
         <v>6626.04</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -711,11 +731,11 @@
         <v>8119.58</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -729,10 +749,10 @@
         <v>13572.82</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -746,10 +766,10 @@
         <v>1172.82</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -763,10 +783,10 @@
         <v>9264.3799999999992</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -780,10 +800,10 @@
         <v>5481.25</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -797,10 +817,10 @@
         <v>13572.82</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -814,10 +834,10 @@
         <v>1172.82</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -831,10 +851,10 @@
         <v>9264.3799999999992</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -848,10 +868,10 @@
         <v>5481.25</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -868,9 +888,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="6">
         <v>70.099999999999994</v>
@@ -882,57 +902,86 @@
         <v>7374.32</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="15">
+        <v>4337.49</v>
+      </c>
+      <c r="C17" s="15">
+        <v>5291.13</v>
+      </c>
+      <c r="D17" s="6">
+        <v>7372.82</v>
+      </c>
       <c r="E17" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="15">
+        <v>1698.27</v>
+      </c>
+      <c r="C18" s="15">
+        <v>6407.89</v>
+      </c>
+      <c r="D18" s="15">
+        <v>6772.82</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="15">
+        <v>1698.27</v>
+      </c>
+      <c r="C19" s="15">
+        <v>6407.89</v>
+      </c>
+      <c r="D19" s="14">
+        <v>7972.82</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="10" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E21" s="3"/>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C23" s="13"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M27" s="8"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D30" s="7"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E22" s="3"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C24" s="13"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M28" s="8"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D31" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prop e estabilidade vertical
</commit_message>
<xml_diff>
--- a/Estabilidade/Centros_Geometricos.xlsx
+++ b/Estabilidade/Centros_Geometricos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Origem</t>
   </si>
@@ -113,12 +113,6 @@
     <t>Components</t>
   </si>
   <si>
-    <t>Tanque Combustivel asa direita</t>
-  </si>
-  <si>
-    <t>Tanque Combustivel asa esquerda</t>
-  </si>
-  <si>
     <t>Fuselagem + Crew + Passengers + Payload</t>
   </si>
   <si>
@@ -138,13 +132,19 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Antigo (Penultimo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanque Combustivel </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,17 +168,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +182,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -283,11 +286,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -314,16 +330,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -344,6 +354,29 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,7 +414,7 @@
         <xdr:cNvPr id="2" name="Imagem 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0437E8A4-EC7B-4CA9-995F-68716B93FCC1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0437E8A4-EC7B-4CA9-995F-68716B93FCC1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -676,7 +709,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,10 +720,11 @@
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="30" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -706,7 +740,7 @@
         <v>21</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -726,48 +760,48 @@
         <v>19</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5">
-        <v>886.68100000000004</v>
+        <v>777.72699999999998</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
       </c>
       <c r="D3" s="5">
-        <v>122.473</v>
+        <v>120.015</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5">
-        <v>4930.6480000000001</v>
+        <v>5496.2160000000003</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
       </c>
       <c r="D4" s="5">
-        <v>-585.29999999999995</v>
+        <v>-675.48299999999995</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -775,10 +809,12 @@
         <v>5</v>
       </c>
       <c r="B5" s="5">
-        <v>1710.99</v>
+        <f>1710.99+479-180-290</f>
+        <v>1719.9899999999998</v>
       </c>
       <c r="C5" s="5">
-        <v>6894.12</v>
+        <f>6894.12 + 269 -150</f>
+        <v>7013.12</v>
       </c>
       <c r="D5" s="5">
         <v>13572.82</v>
@@ -787,7 +823,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -795,10 +831,12 @@
         <v>6</v>
       </c>
       <c r="B6" s="5">
-        <v>1710.99</v>
+        <f>1710.99+479-180-290</f>
+        <v>1719.9899999999998</v>
       </c>
       <c r="C6" s="5">
-        <v>6894.12</v>
+        <f>6894.12 + 269 -150</f>
+        <v>7013.12</v>
       </c>
       <c r="D6" s="5">
         <v>1172.82</v>
@@ -807,7 +845,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -815,21 +853,22 @@
         <v>7</v>
       </c>
       <c r="B7" s="5">
-        <f>5974.32</f>
-        <v>5974.32</v>
+        <f>5974.32+736-50</f>
+        <v>6660.32</v>
       </c>
       <c r="C7" s="5">
-        <v>6894.12</v>
+        <f>6894.12 + 269 -150</f>
+        <v>7013.12</v>
       </c>
       <c r="D7" s="5">
-        <f>9264.38 + 300</f>
-        <v>9564.3799999999992</v>
+        <f>9264.38 + 300 + 789 +170</f>
+        <v>10523.38</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -837,21 +876,22 @@
         <v>8</v>
       </c>
       <c r="B8" s="5">
-        <f>5974.32</f>
-        <v>5974.32</v>
+        <f>5974.32+736-50</f>
+        <v>6660.32</v>
       </c>
       <c r="C8" s="5">
-        <v>6894.12</v>
+        <f>6894.12 + 269 -150</f>
+        <v>7013.12</v>
       </c>
       <c r="D8" s="5">
-        <f>5481.25 - 300</f>
-        <v>5181.25</v>
+        <f>5481.25 - 300 - 789-170</f>
+        <v>4222.25</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -859,10 +899,12 @@
         <v>9</v>
       </c>
       <c r="B9" s="5">
-        <v>1710.99</v>
+        <f>1710.99+479-180-290</f>
+        <v>1719.9899999999998</v>
       </c>
       <c r="C9" s="5">
-        <v>6485.84</v>
+        <f>6485.84+56.49</f>
+        <v>6542.33</v>
       </c>
       <c r="D9" s="5">
         <v>13572.82</v>
@@ -871,7 +913,7 @@
         <v>23</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -879,10 +921,12 @@
         <v>10</v>
       </c>
       <c r="B10" s="5">
-        <v>1710.99</v>
+        <f>1710.99+479-180-290</f>
+        <v>1719.9899999999998</v>
       </c>
       <c r="C10" s="5">
-        <v>6485.84</v>
+        <f>6485.84+56.49</f>
+        <v>6542.33</v>
       </c>
       <c r="D10" s="5">
         <v>1172.82</v>
@@ -891,7 +935,7 @@
         <v>23</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -899,50 +943,52 @@
         <v>11</v>
       </c>
       <c r="B11" s="5">
-        <f>5974.32</f>
-        <v>5974.32</v>
+        <f>5974.32+736-50</f>
+        <v>6660.32</v>
       </c>
       <c r="C11" s="5">
-        <v>6553.33</v>
+        <f>6553.33 + 219 -150-80</f>
+        <v>6542.33</v>
       </c>
       <c r="D11" s="5">
-        <f>9264.38 + 300</f>
-        <v>9564.3799999999992</v>
+        <f>9264.38 + 300 + 789 +170</f>
+        <v>10523.38</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="17">
-        <f>5974.32</f>
-        <v>5974.32</v>
+      <c r="B12" s="5">
+        <f>5974.32+736-50</f>
+        <v>6660.32</v>
       </c>
       <c r="C12" s="5">
-        <v>6553.33</v>
+        <f>6553.33 + 219 -150-80</f>
+        <v>6542.33</v>
       </c>
       <c r="D12" s="5">
-        <f>5481.25 - 300</f>
-        <v>5181.25</v>
+        <f>5481.25 - 300 - 789-170</f>
+        <v>4222.25</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="15">
         <v>-2512.11</v>
       </c>
       <c r="C13" s="5">
@@ -955,37 +1001,38 @@
         <v>13</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="5">
-        <v>1270.0999999999999</v>
+        <f>1270.1 +1081.53</f>
+        <v>2351.63</v>
       </c>
       <c r="C14" s="11">
         <v>4919.6499999999996</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="17">
         <v>7372.82</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="16" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="12">
         <v>4337.49</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="12">
         <v>5291.13</v>
       </c>
       <c r="D15" s="5">
@@ -995,93 +1042,93 @@
         <v>24</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="13">
-        <v>1698.27</v>
-      </c>
-      <c r="C16" s="13">
-        <v>6407.89</v>
-      </c>
-      <c r="D16" s="13">
-        <v>6772.82</v>
+        <v>37</v>
+      </c>
+      <c r="B16" s="12">
+        <v>4337.49</v>
+      </c>
+      <c r="C16" s="12">
+        <f>5291.13 + 820</f>
+        <v>6111.13</v>
+      </c>
+      <c r="D16" s="5">
+        <v>7372.82</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="13">
-        <v>1698.27</v>
-      </c>
-      <c r="C17" s="13">
-        <v>6407.89</v>
-      </c>
-      <c r="D17" s="12">
-        <v>7972.82</v>
+        <v>14</v>
+      </c>
+      <c r="B17" s="10">
+        <v>-1612.11</v>
+      </c>
+      <c r="C17" s="10">
+        <v>4891.13</v>
+      </c>
+      <c r="D17" s="13">
+        <v>7372.82</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="10">
-        <v>-1612.11</v>
-      </c>
-      <c r="C18" s="10">
-        <v>4891.13</v>
-      </c>
-      <c r="D18" s="14">
-        <v>7372.82</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C20" s="22"/>
+      <c r="C20" s="20"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="20"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="18"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="21"/>
+        <v>35</v>
+      </c>
+      <c r="D23" s="19"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="11"/>
-      <c r="G24" s="6"/>
+      <c r="A24" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="27">
+        <v>1270.0999999999999</v>
+      </c>
+      <c r="C24" s="28">
+        <v>4919.6499999999996</v>
+      </c>
+      <c r="D24" s="29">
+        <v>7372.82</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
@@ -1091,83 +1138,83 @@
       <c r="M28" s="7"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="23">
         <v>1844.66</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="23">
         <v>6366.01</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="23">
         <v>9529.07</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="9" t="s">
-        <v>33</v>
+      <c r="F29" s="24" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="23">
         <v>1844.83</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="23">
         <v>6365.9</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="23">
         <v>5213.58</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="9" t="s">
-        <v>33</v>
+      <c r="F30" s="24" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="23">
         <v>5785.74</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="23">
         <v>6031.06</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="23">
         <v>6626.04</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F31" s="9" t="s">
-        <v>33</v>
+      <c r="F31" s="24" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="23">
         <v>5786.01</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="23">
         <v>6031.06</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="23">
         <v>8119.58</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F32" s="9" t="s">
-        <v>33</v>
+      <c r="F32" s="24" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>